<commit_message>
Enviando para o git hub teste de mesa e alguns exercícios corrigidos
</commit_message>
<xml_diff>
--- a/Teste de Mesa/Teste de Mesa.xlsx
+++ b/Teste de Mesa/Teste de Mesa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Desktop\Tarefa 1 - Java\Teste de Mesa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABAE9F2-82CB-4620-9F64-0A133C232832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9528832-C7D5-4F08-8AB6-78B9E18EF9FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{5FD6AB69-EE58-49EA-92E4-9021CC26BC9D}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="7" activeTab="8" xr2:uid="{5FD6AB69-EE58-49EA-92E4-9021CC26BC9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Questão 1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,9 @@
     <sheet name="Questão 4" sheetId="6" r:id="rId4"/>
     <sheet name="Questão 5" sheetId="7" r:id="rId5"/>
     <sheet name="Questão 6" sheetId="8" r:id="rId6"/>
+    <sheet name="Questão 7" sheetId="9" r:id="rId7"/>
+    <sheet name="Questão 8" sheetId="10" r:id="rId8"/>
+    <sheet name="Questão 9" sheetId="11" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
   <si>
     <t>idade</t>
   </si>
@@ -140,6 +143,36 @@
   </si>
   <si>
     <t>TESTE DE MESA QUESTÃO 6</t>
+  </si>
+  <si>
+    <t>num</t>
+  </si>
+  <si>
+    <t>mensagem</t>
+  </si>
+  <si>
+    <t>É MAIOR QUE 10</t>
+  </si>
+  <si>
+    <t>NÃO É MAIOR QUE 10</t>
+  </si>
+  <si>
+    <t>TESTE DE MESA QUESTÃO 7</t>
+  </si>
+  <si>
+    <t>TESTE DE MESA QUESTÃO 8</t>
+  </si>
+  <si>
+    <t>Número positivo !</t>
+  </si>
+  <si>
+    <t>Número negativo !</t>
+  </si>
+  <si>
+    <t>TESTE DE MESA QUESTÃO 9</t>
+  </si>
+  <si>
+    <t>quantMaca</t>
   </si>
 </sst>
 </file>
@@ -211,19 +244,19 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -572,12 +605,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="19.95" customHeight="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
     </row>
     <row r="2" spans="1:4" s="2" customFormat="1" ht="19.95" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -634,15 +667,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.95" customHeight="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -718,15 +751,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.95" customHeight="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -787,15 +820,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.95" customHeight="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -856,15 +889,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.95" customHeight="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -896,7 +929,7 @@
       <c r="D3" s="1">
         <v>300</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>4500</v>
       </c>
       <c r="F3" s="3"/>
@@ -915,7 +948,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A83F9214-FAC2-44F4-B749-EE6235CD81F8}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="63" zoomScaleNormal="63" workbookViewId="0">
+    <sheetView zoomScale="63" zoomScaleNormal="63" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -930,44 +963,275 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.95" customHeight="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="7"/>
+      <c r="D2" s="8"/>
     </row>
     <row r="3" spans="1:7" ht="19.95" customHeight="1">
-      <c r="A3" s="8">
+      <c r="A3" s="7">
         <v>160</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8">
+      <c r="B3" s="7"/>
+      <c r="C3" s="7">
         <v>71.11</v>
       </c>
-      <c r="D3" s="8"/>
+      <c r="D3" s="7"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" ht="19.95" customHeight="1">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7DEE3F0-00D0-4CF3-9E47-C19CA0495BC2}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView zoomScale="63" zoomScaleNormal="63" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="19.95" customHeight="1"/>
+  <cols>
+    <col min="1" max="3" width="20.77734375" style="1"/>
+    <col min="4" max="4" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="20.77734375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="19.95" customHeight="1">
+      <c r="A1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1">
+      <c r="A2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="8"/>
+    </row>
+    <row r="3" spans="1:7" ht="19.95" customHeight="1">
+      <c r="A3" s="7">
+        <v>7</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" ht="19.95" customHeight="1">
+      <c r="A4" s="7">
+        <v>11</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A44E51FA-4447-47AD-A97E-5F5B3379A2B9}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView zoomScale="63" zoomScaleNormal="63" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="19.95" customHeight="1"/>
+  <cols>
+    <col min="1" max="3" width="20.77734375" style="1"/>
+    <col min="4" max="4" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="20.77734375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="19.95" customHeight="1">
+      <c r="A1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1">
+      <c r="A2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="8"/>
+    </row>
+    <row r="3" spans="1:7" ht="19.95" customHeight="1">
+      <c r="A3" s="7">
+        <v>10</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" ht="19.95" customHeight="1">
+      <c r="A4" s="7">
+        <v>-7</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B969D6C5-341E-4AE7-978B-D889046523C4}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="63" zoomScaleNormal="63" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="19.95" customHeight="1"/>
+  <cols>
+    <col min="1" max="3" width="20.77734375" style="1"/>
+    <col min="4" max="4" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="20.77734375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="19.95" customHeight="1">
+      <c r="A1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1">
+      <c r="A2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="8"/>
+    </row>
+    <row r="3" spans="1:7" ht="19.95" customHeight="1">
+      <c r="A3" s="7">
+        <v>6</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7">
+        <v>7.8</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" ht="19.95" customHeight="1">
+      <c r="A4" s="7">
+        <v>12</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7">
+        <v>12</v>
+      </c>
+      <c r="D4" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
Inserindo mais teste de mesas
</commit_message>
<xml_diff>
--- a/Teste de Mesa/Teste de Mesa.xlsx
+++ b/Teste de Mesa/Teste de Mesa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Desktop\Tarefa 1 - Java\Teste de Mesa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9528832-C7D5-4F08-8AB6-78B9E18EF9FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A32FF6A-7399-4D73-A7B0-D86B3689CC37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="7" activeTab="8" xr2:uid="{5FD6AB69-EE58-49EA-92E4-9021CC26BC9D}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="11" activeTab="12" xr2:uid="{5FD6AB69-EE58-49EA-92E4-9021CC26BC9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Questão 1" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,10 @@
     <sheet name="Questão 7" sheetId="9" r:id="rId7"/>
     <sheet name="Questão 8" sheetId="10" r:id="rId8"/>
     <sheet name="Questão 9" sheetId="11" r:id="rId9"/>
+    <sheet name="Questão 10" sheetId="12" r:id="rId10"/>
+    <sheet name="Questão 11" sheetId="13" r:id="rId11"/>
+    <sheet name="Questão 12" sheetId="14" r:id="rId12"/>
+    <sheet name="Questão 13" sheetId="16" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="61">
   <si>
     <t>idade</t>
   </si>
@@ -173,6 +177,60 @@
   </si>
   <si>
     <t>quantMaca</t>
+  </si>
+  <si>
+    <t>TESTE DE MESA QUESTÃO 10</t>
+  </si>
+  <si>
+    <t>nota1</t>
+  </si>
+  <si>
+    <t>nota2</t>
+  </si>
+  <si>
+    <t>media</t>
+  </si>
+  <si>
+    <t>Aluno foi Aprovado!</t>
+  </si>
+  <si>
+    <t>Aluno não foi Aprovado!</t>
+  </si>
+  <si>
+    <t>anoAtual</t>
+  </si>
+  <si>
+    <t>anoNascimento</t>
+  </si>
+  <si>
+    <t>votar</t>
+  </si>
+  <si>
+    <t>Pode votar este ano!</t>
+  </si>
+  <si>
+    <t>Não pode votar este ano!</t>
+  </si>
+  <si>
+    <t>TESTE DE MESA QUESTÃO 11</t>
+  </si>
+  <si>
+    <t>TESTE DE MESA QUESTÃO 12</t>
+  </si>
+  <si>
+    <t>num1</t>
+  </si>
+  <si>
+    <t>num2</t>
+  </si>
+  <si>
+    <t>"Os números não podem ser iguais"</t>
+  </si>
+  <si>
+    <t>"Não pode ser lido valores iguais"</t>
+  </si>
+  <si>
+    <t>TESTE DE MESA QUESTÃO 13</t>
   </si>
 </sst>
 </file>
@@ -233,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -258,6 +316,27 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -649,6 +728,354 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B602F9EF-D7D5-474E-B616-DAC39547A554}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="19.95" customHeight="1"/>
+  <cols>
+    <col min="1" max="3" width="20.77734375" style="11"/>
+    <col min="4" max="4" width="23.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.77734375" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="20.77734375" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="19.95" customHeight="1">
+      <c r="A1" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+    </row>
+    <row r="2" spans="1:7" s="12" customFormat="1" ht="19.95" customHeight="1">
+      <c r="A2" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="19.95" customHeight="1">
+      <c r="A3" s="11">
+        <v>10</v>
+      </c>
+      <c r="B3" s="11">
+        <v>10</v>
+      </c>
+      <c r="C3" s="11">
+        <f>(A3+B3)/2</f>
+        <v>10</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+    </row>
+    <row r="4" spans="1:7" ht="19.95" customHeight="1">
+      <c r="A4" s="11">
+        <v>6</v>
+      </c>
+      <c r="B4" s="11">
+        <v>2</v>
+      </c>
+      <c r="C4" s="11">
+        <f>(A4+B4)/2</f>
+        <v>4</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{894E255A-D771-49A1-9576-54E6C11B2731}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="19.95" customHeight="1"/>
+  <cols>
+    <col min="1" max="3" width="20.77734375" style="11"/>
+    <col min="4" max="4" width="23.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.77734375" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="20.77734375" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="19.95" customHeight="1">
+      <c r="A1" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+    </row>
+    <row r="2" spans="1:7" s="12" customFormat="1" ht="19.95" customHeight="1">
+      <c r="A2" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="19.95" customHeight="1">
+      <c r="A3" s="11">
+        <v>2025</v>
+      </c>
+      <c r="B3" s="11">
+        <v>2005</v>
+      </c>
+      <c r="C3" s="11">
+        <f>A3-B3</f>
+        <v>20</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+    </row>
+    <row r="4" spans="1:7" ht="19.95" customHeight="1">
+      <c r="A4" s="11">
+        <v>2025</v>
+      </c>
+      <c r="B4" s="11">
+        <v>2010</v>
+      </c>
+      <c r="C4" s="11">
+        <f>A4-B4</f>
+        <v>15</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35DD0FE3-9385-4C84-B97B-331874C74DBA}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="19.95" customHeight="1"/>
+  <cols>
+    <col min="1" max="3" width="20.77734375" style="11"/>
+    <col min="4" max="4" width="23.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.77734375" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="20.77734375" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="19.95" customHeight="1">
+      <c r="A1" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+    </row>
+    <row r="2" spans="1:7" s="12" customFormat="1" ht="19.95" customHeight="1">
+      <c r="A2" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="14"/>
+    </row>
+    <row r="3" spans="1:7" ht="19.95" customHeight="1">
+      <c r="A3" s="11">
+        <v>2000</v>
+      </c>
+      <c r="B3" s="11">
+        <v>2000</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="15"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+    </row>
+    <row r="4" spans="1:7" ht="19.95" customHeight="1">
+      <c r="A4" s="11">
+        <v>15</v>
+      </c>
+      <c r="B4" s="11">
+        <v>20</v>
+      </c>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+    </row>
+    <row r="5" spans="1:7" ht="19.95" customHeight="1">
+      <c r="A5" s="11">
+        <v>7</v>
+      </c>
+      <c r="B5" s="11">
+        <v>10</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2CB8F11-F887-4492-88E4-4D87D4AED7FC}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="19.95" customHeight="1"/>
+  <cols>
+    <col min="1" max="3" width="20.77734375" style="11"/>
+    <col min="4" max="4" width="23.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.77734375" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="20.77734375" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="19.95" customHeight="1">
+      <c r="A1" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+    </row>
+    <row r="2" spans="1:7" s="12" customFormat="1" ht="19.95" customHeight="1">
+      <c r="A2" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="14"/>
+    </row>
+    <row r="3" spans="1:7" ht="19.95" customHeight="1">
+      <c r="A3" s="11">
+        <v>10</v>
+      </c>
+      <c r="B3" s="11">
+        <v>10</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="15"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+    </row>
+    <row r="4" spans="1:7" ht="19.95" customHeight="1">
+      <c r="A4" s="11">
+        <v>7</v>
+      </c>
+      <c r="B4" s="11">
+        <v>8</v>
+      </c>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+    </row>
+    <row r="5" spans="1:7" ht="19.95" customHeight="1">
+      <c r="A5" s="11">
+        <v>10</v>
+      </c>
+      <c r="B5" s="11">
+        <v>3</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{161DCB8E-B926-4A68-B823-DCD347A28F24}">
   <dimension ref="A1:G3"/>
@@ -1175,7 +1602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B969D6C5-341E-4AE7-978B-D889046523C4}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="63" zoomScaleNormal="63" workbookViewId="0">
+    <sheetView zoomScale="63" zoomScaleNormal="63" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Entrega final dos testes de mesas e correção
</commit_message>
<xml_diff>
--- a/Teste de Mesa/Teste de Mesa.xlsx
+++ b/Teste de Mesa/Teste de Mesa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Desktop\Tarefa 1 - Java\Teste de Mesa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35ADC833-B673-431C-8FC8-D99EBE230D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132852B2-6347-4D92-9CCA-8FECA90B67E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5FD6AB69-EE58-49EA-92E4-9021CC26BC9D}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="15" activeTab="16" xr2:uid="{5FD6AB69-EE58-49EA-92E4-9021CC26BC9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Questão 1" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="93">
   <si>
     <t>idade</t>
   </si>
@@ -316,6 +316,21 @@
   </si>
   <si>
     <t>api</t>
+  </si>
+  <si>
+    <t>Rodrigo</t>
+  </si>
+  <si>
+    <t>"O número 20 é maior que 15"</t>
+  </si>
+  <si>
+    <t>"O número 10 é maior que 7 "</t>
+  </si>
+  <si>
+    <t>"7,  8"</t>
+  </si>
+  <si>
+    <t>"3,  10"</t>
   </si>
 </sst>
 </file>
@@ -325,7 +340,7 @@
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -437,20 +452,20 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -460,475 +475,24 @@
   </cellStyles>
   <dxfs count="98">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Ariall"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Ariall"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Ariall"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Ariall"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Ariall"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Ariall"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Ariall"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Ariall"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Ariall"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Ariall"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Ariall"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Ariall"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Ariall"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Ariall"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <name val="Ariall"/>
-        <scheme val="none"/>
-      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -952,20 +516,38 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Ariall"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -988,31 +570,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1038,6 +599,460 @@
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Ariall"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Ariall"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Ariall"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Ariall"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Ariall"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Ariall"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Ariall"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Ariall"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Ariall"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Ariall"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Ariall"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Ariall"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Ariall"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Ariall"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1052,79 +1067,79 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{457E9B23-898C-47A5-9E35-474EB58855A4}" name="Tabela18" displayName="Tabela18" ref="A2:D3" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="A2:D3" xr:uid="{457E9B23-898C-47A5-9E35-474EB58855A4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{457E9B23-898C-47A5-9E35-474EB58855A4}" name="Tabela18" displayName="Tabela18" ref="A2:D4" totalsRowShown="0" headerRowDxfId="97" dataDxfId="96">
+  <autoFilter ref="A2:D4" xr:uid="{457E9B23-898C-47A5-9E35-474EB58855A4}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{2C94D44A-9F4E-40AA-8D2F-1B28C2E834F7}" name="idade" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{63E3A8EF-9564-4FA7-8575-77DE8321A846}" name="meses" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{9D9B753D-0A1C-4A27-9916-3E951D2059F1}" name="dia" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{E53C847E-C687-4B84-8FA7-53557C6DF1F1}" name="TotalDias" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{2C94D44A-9F4E-40AA-8D2F-1B28C2E834F7}" name="idade" dataDxfId="95"/>
+    <tableColumn id="2" xr3:uid="{63E3A8EF-9564-4FA7-8575-77DE8321A846}" name="meses" dataDxfId="94"/>
+    <tableColumn id="3" xr3:uid="{9D9B753D-0A1C-4A27-9916-3E951D2059F1}" name="dia" dataDxfId="93"/>
+    <tableColumn id="4" xr3:uid="{E53C847E-C687-4B84-8FA7-53557C6DF1F1}" name="TotalDias" dataDxfId="92"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{51F9150F-DD38-465C-BADB-03B2EC935F65}" name="Tabela9" displayName="Tabela9" ref="A2:D4" totalsRowShown="0" headerRowDxfId="50" dataDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{51F9150F-DD38-465C-BADB-03B2EC935F65}" name="Tabela9" displayName="Tabela9" ref="A2:D4" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
   <autoFilter ref="A2:D4" xr:uid="{51F9150F-DD38-465C-BADB-03B2EC935F65}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{5773977A-794E-4961-BCE9-E8F162886D7A}" name="nota1" dataDxfId="55"/>
-    <tableColumn id="2" xr3:uid="{401DD383-0744-41E0-9A11-77E8C8C9796A}" name="nota2" dataDxfId="54"/>
-    <tableColumn id="3" xr3:uid="{51FD8612-E240-43C0-854C-4C9CFD455C6D}" name="media" dataDxfId="53">
+    <tableColumn id="1" xr3:uid="{5773977A-794E-4961-BCE9-E8F162886D7A}" name="nota1" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{401DD383-0744-41E0-9A11-77E8C8C9796A}" name="nota2" dataDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{51FD8612-E240-43C0-854C-4C9CFD455C6D}" name="media" dataDxfId="43">
       <calculatedColumnFormula>(A3+B3)/2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{9A6920EF-7A06-47EC-93F6-90078EA72275}" name="mensagem" dataDxfId="52"/>
+    <tableColumn id="4" xr3:uid="{9A6920EF-7A06-47EC-93F6-90078EA72275}" name="mensagem" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{3351B7EC-1E6F-4D0C-B2FB-D650C490FAC0}" name="Tabela8" displayName="Tabela8" ref="A2:D4" totalsRowShown="0" headerRowDxfId="56" dataDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{3351B7EC-1E6F-4D0C-B2FB-D650C490FAC0}" name="Tabela8" displayName="Tabela8" ref="A2:D4" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
   <autoFilter ref="A2:D4" xr:uid="{3351B7EC-1E6F-4D0C-B2FB-D650C490FAC0}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{82C06D3B-0FB5-49EF-9D26-4DB43E7386E1}" name="anoAtual" dataDxfId="61"/>
-    <tableColumn id="2" xr3:uid="{03DEF9D4-CB62-4C8B-A480-F9A98D75D4D6}" name="anoNascimento" dataDxfId="60"/>
-    <tableColumn id="3" xr3:uid="{01437B17-CD91-4521-9ABB-3928FEDD63C9}" name="votar" dataDxfId="59">
+    <tableColumn id="1" xr3:uid="{82C06D3B-0FB5-49EF-9D26-4DB43E7386E1}" name="anoAtual" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{03DEF9D4-CB62-4C8B-A480-F9A98D75D4D6}" name="anoNascimento" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{01437B17-CD91-4521-9ABB-3928FEDD63C9}" name="votar" dataDxfId="37">
       <calculatedColumnFormula>A3-B3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C36CCADF-76EA-47BE-821F-0AEDA1F512E8}" name="mensagem" dataDxfId="58"/>
+    <tableColumn id="4" xr3:uid="{C36CCADF-76EA-47BE-821F-0AEDA1F512E8}" name="mensagem" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{BF403AD1-5AF5-4D6C-9C56-88AC960AD96E}" name="Tabela7" displayName="Tabela7" ref="A2:C5" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{BF403AD1-5AF5-4D6C-9C56-88AC960AD96E}" name="Tabela7" displayName="Tabela7" ref="A2:C5" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="A2:C5" xr:uid="{BF403AD1-5AF5-4D6C-9C56-88AC960AD96E}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{EF22F0F2-9CC6-4918-9DFE-340EE18DD356}" name="num1" dataDxfId="66"/>
-    <tableColumn id="2" xr3:uid="{53A8B66C-5B9B-4D2D-BC36-FC94A620019C}" name="num2" dataDxfId="65"/>
-    <tableColumn id="3" xr3:uid="{CBD6E5EF-70E5-4E3A-9F37-27334FB6A222}" name="mensagem" dataDxfId="64"/>
+    <tableColumn id="1" xr3:uid="{EF22F0F2-9CC6-4918-9DFE-340EE18DD356}" name="num1" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{53A8B66C-5B9B-4D2D-BC36-FC94A620019C}" name="num2" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{CBD6E5EF-70E5-4E3A-9F37-27334FB6A222}" name="mensagem" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E5850A33-6221-4A46-96ED-FF10D0004FA3}" name="Tabela6" displayName="Tabela6" ref="A2:C5" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E5850A33-6221-4A46-96ED-FF10D0004FA3}" name="Tabela6" displayName="Tabela6" ref="A2:C5" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
   <autoFilter ref="A2:C5" xr:uid="{E5850A33-6221-4A46-96ED-FF10D0004FA3}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{D9488621-2465-43DB-912B-003437FD7952}" name="num1" dataDxfId="71"/>
-    <tableColumn id="2" xr3:uid="{DFF62B29-81AA-41C0-AF67-E2F0D1770395}" name="num2" dataDxfId="70"/>
-    <tableColumn id="3" xr3:uid="{7904F671-7521-4627-A24B-252C72D712FF}" name="mensagem" dataDxfId="69"/>
+    <tableColumn id="1" xr3:uid="{D9488621-2465-43DB-912B-003437FD7952}" name="num1" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{DFF62B29-81AA-41C0-AF67-E2F0D1770395}" name="num2" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{7904F671-7521-4627-A24B-252C72D712FF}" name="mensagem" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{F0B0830A-5654-4A82-B80C-E21A26F40EB8}" name="Tabela5" displayName="Tabela5" ref="A2:C4" totalsRowShown="0" headerRowDxfId="72" dataDxfId="73">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{F0B0830A-5654-4A82-B80C-E21A26F40EB8}" name="Tabela5" displayName="Tabela5" ref="A2:C4" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <autoFilter ref="A2:C4" xr:uid="{F0B0830A-5654-4A82-B80C-E21A26F40EB8}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{01A7E088-9E92-4381-9848-0575454FEB9D}" name="horaInicio" dataDxfId="76"/>
-    <tableColumn id="2" xr3:uid="{1C65E772-FF3D-457C-B889-5D319E938204}" name="horaFim" dataDxfId="75"/>
-    <tableColumn id="3" xr3:uid="{DFA3E247-CEFD-4F84-A99B-EB9EE56868BE}" name="totalHoras" dataDxfId="74"/>
+    <tableColumn id="1" xr3:uid="{01A7E088-9E92-4381-9848-0575454FEB9D}" name="horaInicio" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{1C65E772-FF3D-457C-B889-5D319E938204}" name="horaFim" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{DFA3E247-CEFD-4F84-A99B-EB9EE56868BE}" name="totalHoras" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1134,9 +1149,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D25D7836-27B4-4BD8-8EF6-8DCB69289D0F}" name="Tabela4" displayName="Tabela4" ref="A2:D4" totalsRowShown="0">
   <autoFilter ref="A2:D4" xr:uid="{D25D7836-27B4-4BD8-8EF6-8DCB69289D0F}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{11A7A83A-469C-4521-8691-9EF105155692}" name="horas" dataDxfId="79"/>
-    <tableColumn id="2" xr3:uid="{8135D432-4B7F-401F-A515-5F324ECD519F}" name="salHora" dataDxfId="78"/>
-    <tableColumn id="3" xr3:uid="{E65DE681-381B-4E94-B240-A7B3A22D82CB}" name="salTotal" dataDxfId="77">
+    <tableColumn id="1" xr3:uid="{11A7A83A-469C-4521-8691-9EF105155692}" name="horas" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{8135D432-4B7F-401F-A515-5F324ECD519F}" name="salHora" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{E65DE681-381B-4E94-B240-A7B3A22D82CB}" name="salTotal" dataDxfId="18">
       <calculatedColumnFormula>(B3*A3)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{A23112CB-CC94-449F-85D3-875A29ED524B}" name="acresimo">
@@ -1148,16 +1163,16 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1AF5DCC8-B196-4E52-B82F-9147C448DA12}" name="Tabela3" displayName="Tabela3" ref="A2:E3" totalsRowShown="0" headerRowDxfId="80">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1AF5DCC8-B196-4E52-B82F-9147C448DA12}" name="Tabela3" displayName="Tabela3" ref="A2:E3" totalsRowShown="0" headerRowDxfId="17">
   <autoFilter ref="A2:E3" xr:uid="{1AF5DCC8-B196-4E52-B82F-9147C448DA12}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{056055FE-1D85-4E7E-9959-A6F5F4DF5769}" name="jan" dataDxfId="85"/>
-    <tableColumn id="2" xr3:uid="{28981476-EE55-4739-B07E-ECADB89845A6}" name="fev" dataDxfId="84"/>
-    <tableColumn id="3" xr3:uid="{952D6F13-C2E0-4674-8424-DE127E46EE2A}" name="mar" dataDxfId="83"/>
-    <tableColumn id="4" xr3:uid="{B15800BE-2169-4817-A554-B3CD28AB6F26}" name="despesaTotal" dataDxfId="82">
+    <tableColumn id="1" xr3:uid="{056055FE-1D85-4E7E-9959-A6F5F4DF5769}" name="jan" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{28981476-EE55-4739-B07E-ECADB89845A6}" name="fev" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{952D6F13-C2E0-4674-8424-DE127E46EE2A}" name="mar" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{B15800BE-2169-4817-A554-B3CD28AB6F26}" name="despesaTotal" dataDxfId="13">
       <calculatedColumnFormula>A3+B3+C3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{6D42233D-A8F2-4658-84E6-9EF4274185D2}" name="mediaMensal" dataDxfId="81" dataCellStyle="Moeda">
+    <tableColumn id="5" xr3:uid="{6D42233D-A8F2-4658-84E6-9EF4274185D2}" name="mediaMensal" dataDxfId="12" dataCellStyle="Moeda">
       <calculatedColumnFormula>D3/3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1166,116 +1181,116 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0F19B031-C581-41BC-8D37-6074C996883D}" name="Tabela2" displayName="Tabela2" ref="A2:K4" totalsRowShown="0" headerRowDxfId="97">
-  <autoFilter ref="A2:K4" xr:uid="{0F19B031-C581-41BC-8D37-6074C996883D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0F19B031-C581-41BC-8D37-6074C996883D}" name="Tabela2" displayName="Tabela2" ref="A2:K5" totalsRowShown="0" headerRowDxfId="11">
+  <autoFilter ref="A2:K5" xr:uid="{0F19B031-C581-41BC-8D37-6074C996883D}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{AFE554C4-6A33-4F7F-8AEE-8F3E7225C62C}" name="p1" dataDxfId="90"/>
-    <tableColumn id="2" xr3:uid="{829F5414-08A8-467D-A676-BC95B84B7694}" name="e1" dataDxfId="89"/>
-    <tableColumn id="3" xr3:uid="{A925B593-125D-40CA-941C-82D103FC8623}" name="e2" dataDxfId="88"/>
-    <tableColumn id="4" xr3:uid="{636979E3-A504-4760-9E5C-40D672CC404C}" name="x" dataDxfId="86"/>
-    <tableColumn id="5" xr3:uid="{4D297FEA-5C6C-4119-BAE6-E2D155E8E453}" name="media" dataDxfId="87" dataCellStyle="Moeda"/>
-    <tableColumn id="6" xr3:uid="{679309DF-EFC6-40BC-995A-E62BE05FAF16}" name="max" dataDxfId="94" dataCellStyle="Vírgula"/>
-    <tableColumn id="7" xr3:uid="{7F1A63DD-4014-4633-B4E6-EA6E3852569E}" name="fator" dataDxfId="92"/>
-    <tableColumn id="11" xr3:uid="{82091D63-FD1D-4933-81E0-05B5E02D9241}" name="api" dataDxfId="91"/>
-    <tableColumn id="8" xr3:uid="{2149D56E-AED0-4F16-A976-EDC94FE8C323}" name="notaTotal" dataDxfId="93"/>
-    <tableColumn id="9" xr3:uid="{CE038BB0-82BE-4172-8146-B2709E44582F}" name="sub" dataDxfId="96"/>
-    <tableColumn id="10" xr3:uid="{35CE5CFC-1FF1-4823-A7DB-C28CF8D7B1F7}" name="notaSubTotal" dataDxfId="95"/>
+    <tableColumn id="1" xr3:uid="{AFE554C4-6A33-4F7F-8AEE-8F3E7225C62C}" name="p1" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{829F5414-08A8-467D-A676-BC95B84B7694}" name="e1" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{A925B593-125D-40CA-941C-82D103FC8623}" name="e2" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{636979E3-A504-4760-9E5C-40D672CC404C}" name="x" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{4D297FEA-5C6C-4119-BAE6-E2D155E8E453}" name="media" dataDxfId="6" dataCellStyle="Moeda"/>
+    <tableColumn id="6" xr3:uid="{679309DF-EFC6-40BC-995A-E62BE05FAF16}" name="max" dataDxfId="5" dataCellStyle="Vírgula"/>
+    <tableColumn id="7" xr3:uid="{7F1A63DD-4014-4633-B4E6-EA6E3852569E}" name="fator" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{82091D63-FD1D-4933-81E0-05B5E02D9241}" name="api" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{2149D56E-AED0-4F16-A976-EDC94FE8C323}" name="notaTotal" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{CE038BB0-82BE-4172-8146-B2709E44582F}" name="sub" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{35CE5CFC-1FF1-4823-A7DB-C28CF8D7B1F7}" name="notaSubTotal" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{70243BE6-2C7A-44C6-8E3B-6D09092F0B59}" name="Tabela17" displayName="Tabela17" ref="A2:G4" totalsRowShown="0" headerRowDxfId="6" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{70243BE6-2C7A-44C6-8E3B-6D09092F0B59}" name="Tabela17" displayName="Tabela17" ref="A2:G4" totalsRowShown="0" headerRowDxfId="91" dataDxfId="90">
   <autoFilter ref="A2:G4" xr:uid="{70243BE6-2C7A-44C6-8E3B-6D09092F0B59}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{6FCDE9B0-A376-4477-A26A-B180B0663DDB}" name="eleitores" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{BD0E5794-8ED1-4EF6-A5A6-ED58DCE73757}" name="votoNulo" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{3EEB9524-CD0F-4188-A3DB-7EDFBBC672E8}" name="votoBranco" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{683A594D-5544-4A6C-86A7-6FDBB5A3E343}" name="votoValido" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{0637594B-8DC2-43E4-9CD2-5410DD4A3F4A}" name="percentualVotoNulo" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{7DA407F4-94DA-40E6-98D6-850D50D6A7D3}" name="percentualVotoBranco" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{72CD1ABF-C664-4D95-AEB4-8A39EDC06BDE}" name="percentualVotoValido" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{6FCDE9B0-A376-4477-A26A-B180B0663DDB}" name="eleitores" dataDxfId="89"/>
+    <tableColumn id="2" xr3:uid="{BD0E5794-8ED1-4EF6-A5A6-ED58DCE73757}" name="votoNulo" dataDxfId="88"/>
+    <tableColumn id="3" xr3:uid="{3EEB9524-CD0F-4188-A3DB-7EDFBBC672E8}" name="votoBranco" dataDxfId="87"/>
+    <tableColumn id="4" xr3:uid="{683A594D-5544-4A6C-86A7-6FDBB5A3E343}" name="votoValido" dataDxfId="86"/>
+    <tableColumn id="5" xr3:uid="{0637594B-8DC2-43E4-9CD2-5410DD4A3F4A}" name="percentualVotoNulo" dataDxfId="85"/>
+    <tableColumn id="6" xr3:uid="{7DA407F4-94DA-40E6-98D6-850D50D6A7D3}" name="percentualVotoBranco" dataDxfId="84"/>
+    <tableColumn id="7" xr3:uid="{72CD1ABF-C664-4D95-AEB4-8A39EDC06BDE}" name="percentualVotoValido" dataDxfId="83"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{CAA7507C-32F1-456E-AAFF-390F12C9291B}" name="Tabela16" displayName="Tabela16" ref="A2:D3" totalsRowShown="0" headerRowDxfId="15" dataDxfId="16">
-  <autoFilter ref="A2:D3" xr:uid="{CAA7507C-32F1-456E-AAFF-390F12C9291B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{CAA7507C-32F1-456E-AAFF-390F12C9291B}" name="Tabela16" displayName="Tabela16" ref="A2:D4" totalsRowShown="0" headerRowDxfId="82" dataDxfId="81">
+  <autoFilter ref="A2:D4" xr:uid="{CAA7507C-32F1-456E-AAFF-390F12C9291B}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{638D6BF2-B88A-4438-B751-E5DE2D7869E9}" name="nome" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{BB14071C-B0CB-4D4E-87BB-C58456E52FD2}" name="salarioAtual" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{1564F22A-B1F7-407C-8C3F-0025B78F1477}" name="reajuste" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{985BAFA1-CC17-4088-9C20-C4EB9DAA1340}" name="salarioReajustado" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{638D6BF2-B88A-4438-B751-E5DE2D7869E9}" name="nome" dataDxfId="80"/>
+    <tableColumn id="2" xr3:uid="{BB14071C-B0CB-4D4E-87BB-C58456E52FD2}" name="salarioAtual" dataDxfId="79"/>
+    <tableColumn id="3" xr3:uid="{1564F22A-B1F7-407C-8C3F-0025B78F1477}" name="reajuste" dataDxfId="78"/>
+    <tableColumn id="4" xr3:uid="{985BAFA1-CC17-4088-9C20-C4EB9DAA1340}" name="salarioReajustado" dataDxfId="77"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{24E1C70D-B819-4673-BD05-C68D98122002}" name="Tabela15" displayName="Tabela15" ref="A2:D3" totalsRowShown="0" headerRowDxfId="21" dataDxfId="22">
-  <autoFilter ref="A2:D3" xr:uid="{24E1C70D-B819-4673-BD05-C68D98122002}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{24E1C70D-B819-4673-BD05-C68D98122002}" name="Tabela15" displayName="Tabela15" ref="A2:D4" totalsRowShown="0" headerRowDxfId="76" dataDxfId="75">
+  <autoFilter ref="A2:D4" xr:uid="{24E1C70D-B819-4673-BD05-C68D98122002}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{FE0B9877-FF57-4B7E-940F-CDA1FF5B5E9E}" name="distribuidor" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{C72ACDA6-8322-42C5-B55C-881A45327043}" name="imposto" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{639B90A6-CDEE-46C7-A175-DC9FADEA2EC7}" name="custoFabrica" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{8354850E-B3EA-47C9-A1EB-9D80FA1257F9}" name="custoFinal" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{FE0B9877-FF57-4B7E-940F-CDA1FF5B5E9E}" name="distribuidor" dataDxfId="74"/>
+    <tableColumn id="2" xr3:uid="{C72ACDA6-8322-42C5-B55C-881A45327043}" name="imposto" dataDxfId="73"/>
+    <tableColumn id="3" xr3:uid="{639B90A6-CDEE-46C7-A175-DC9FADEA2EC7}" name="custoFabrica" dataDxfId="72"/>
+    <tableColumn id="4" xr3:uid="{8354850E-B3EA-47C9-A1EB-9D80FA1257F9}" name="custoFinal" dataDxfId="71"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{77315783-4666-44B5-9C23-D3A3D74D4934}" name="Tabela14" displayName="Tabela14" ref="A2:E3" totalsRowShown="0" headerRowDxfId="27" dataDxfId="28">
-  <autoFilter ref="A2:E3" xr:uid="{77315783-4666-44B5-9C23-D3A3D74D4934}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{77315783-4666-44B5-9C23-D3A3D74D4934}" name="Tabela14" displayName="Tabela14" ref="A2:E4" totalsRowShown="0" headerRowDxfId="70" dataDxfId="69">
+  <autoFilter ref="A2:E4" xr:uid="{77315783-4666-44B5-9C23-D3A3D74D4934}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{EEE3E0FA-4629-4645-A676-21DC9A091B68}" name="salFixo" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{72DA4698-7C30-4F2F-A6E4-E1CB30405F1F}" name="quantCarro" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{1720923D-6E45-493B-A032-154963DEC6ED}" name="valorVendas" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{81581BE8-3CE8-4485-9271-4AA803E2E9A5}" name="comissao" dataDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{2937ACB6-B611-4306-A9CF-FB3A32837501}" name="total" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{EEE3E0FA-4629-4645-A676-21DC9A091B68}" name="salFixo" dataDxfId="68"/>
+    <tableColumn id="2" xr3:uid="{72DA4698-7C30-4F2F-A6E4-E1CB30405F1F}" name="quantCarro" dataDxfId="67"/>
+    <tableColumn id="3" xr3:uid="{1720923D-6E45-493B-A032-154963DEC6ED}" name="valorVendas" dataDxfId="66"/>
+    <tableColumn id="4" xr3:uid="{81581BE8-3CE8-4485-9271-4AA803E2E9A5}" name="comissao" dataDxfId="65"/>
+    <tableColumn id="5" xr3:uid="{2937ACB6-B611-4306-A9CF-FB3A32837501}" name="total" dataDxfId="64"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{B8D4B782-7F22-485A-A9E1-5295FC66AA42}" name="Tabela13" displayName="Tabela13" ref="A2:B3" totalsRowShown="0" headerRowDxfId="34" dataDxfId="35">
-  <autoFilter ref="A2:B3" xr:uid="{B8D4B782-7F22-485A-A9E1-5295FC66AA42}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{B8D4B782-7F22-485A-A9E1-5295FC66AA42}" name="Tabela13" displayName="Tabela13" ref="A2:B4" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62">
+  <autoFilter ref="A2:B4" xr:uid="{B8D4B782-7F22-485A-A9E1-5295FC66AA42}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{0E1E3D70-C00E-4632-A5D4-38224F74F477}" name="fahrenheit" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{EAA41675-6B69-4136-AF2D-161DDC93178D}" name="celsius" dataDxfId="36"/>
+    <tableColumn id="1" xr3:uid="{0E1E3D70-C00E-4632-A5D4-38224F74F477}" name="fahrenheit" dataDxfId="61"/>
+    <tableColumn id="3" xr3:uid="{EAA41675-6B69-4136-AF2D-161DDC93178D}" name="celsius" dataDxfId="60"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{B1A6E406-50DA-4842-BAC0-A0315502E127}" name="Tabela12" displayName="Tabela12" ref="A2:B4" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{B1A6E406-50DA-4842-BAC0-A0315502E127}" name="Tabela12" displayName="Tabela12" ref="A2:B4" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
   <autoFilter ref="A2:B4" xr:uid="{B1A6E406-50DA-4842-BAC0-A0315502E127}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{254A0562-B52A-4DDF-96B7-D9828F9169BD}" name="num" dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{15581D00-4C2B-4C86-998F-52F2A7C95B8E}" name="mensagem" dataDxfId="38"/>
+    <tableColumn id="1" xr3:uid="{254A0562-B52A-4DDF-96B7-D9828F9169BD}" name="num" dataDxfId="57"/>
+    <tableColumn id="3" xr3:uid="{15581D00-4C2B-4C86-998F-52F2A7C95B8E}" name="mensagem" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{32F0C918-87DF-4000-BF57-767936EA1602}" name="Tabela11" displayName="Tabela11" ref="A2:B4" totalsRowShown="0" headerRowDxfId="42" dataDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{32F0C918-87DF-4000-BF57-767936EA1602}" name="Tabela11" displayName="Tabela11" ref="A2:B4" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
   <autoFilter ref="A2:B4" xr:uid="{32F0C918-87DF-4000-BF57-767936EA1602}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{5CE21FBE-D53C-4DB6-A10B-EF93510FF5BA}" name="num" dataDxfId="45"/>
-    <tableColumn id="3" xr3:uid="{93210568-B566-4FF3-9638-0A6D5B7649B3}" name="mensagem" dataDxfId="44"/>
+    <tableColumn id="1" xr3:uid="{5CE21FBE-D53C-4DB6-A10B-EF93510FF5BA}" name="num" dataDxfId="53"/>
+    <tableColumn id="3" xr3:uid="{93210568-B566-4FF3-9638-0A6D5B7649B3}" name="mensagem" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{BCBE699E-ED1D-4087-9D4C-C090DCF71B23}" name="Tabela10" displayName="Tabela10" ref="A2:B4" totalsRowShown="0" headerRowDxfId="46" dataDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{BCBE699E-ED1D-4087-9D4C-C090DCF71B23}" name="Tabela10" displayName="Tabela10" ref="A2:B4" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
   <autoFilter ref="A2:B4" xr:uid="{BCBE699E-ED1D-4087-9D4C-C090DCF71B23}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{74C6135A-E0CC-42AF-9D15-068B7C417C9F}" name="quantMaca" dataDxfId="49"/>
@@ -1602,10 +1617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{118F7E97-4F50-4DBC-9D7B-A018EDE7BCE2}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="19.95" customHeight="1"/>
@@ -1614,12 +1629,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="19.95" customHeight="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
     </row>
     <row r="2" spans="1:4" s="2" customFormat="1" ht="19.95" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -1647,6 +1662,20 @@
       </c>
       <c r="D3" s="1">
         <v>7017</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="19.95" customHeight="1">
+      <c r="A4" s="1">
+        <v>22</v>
+      </c>
+      <c r="B4" s="1">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1">
+        <v>26</v>
+      </c>
+      <c r="D4" s="1">
+        <v>8326</v>
       </c>
     </row>
   </sheetData>
@@ -1680,12 +1709,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.95" customHeight="1">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -1770,12 +1799,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.95" customHeight="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -1844,7 +1873,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="19.95" customHeight="1"/>
@@ -1858,11 +1887,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19.95" customHeight="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
@@ -1899,16 +1928,20 @@
       <c r="B4" s="1">
         <v>20</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="19.95" customHeight="1">
       <c r="A5" s="1">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1">
         <v>7</v>
       </c>
-      <c r="B5" s="1">
-        <v>10</v>
-      </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>90</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1927,7 +1960,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="19.95" customHeight="1"/>
@@ -1941,11 +1974,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19.95" customHeight="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
@@ -1982,7 +2015,9 @@
       <c r="B4" s="1">
         <v>8</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="19.95" customHeight="1">
       <c r="A5" s="1">
@@ -1991,7 +2026,9 @@
       <c r="B5" s="1">
         <v>3</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>92</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2024,11 +2061,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19.95" customHeight="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
@@ -2089,7 +2126,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="19.95" customHeight="1"/>
@@ -2103,12 +2140,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.95" customHeight="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -2148,15 +2185,15 @@
         <v>180</v>
       </c>
       <c r="B4" s="7">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1">
         <f>(B4*A4)</f>
-        <v>1800</v>
+        <v>2880</v>
       </c>
       <c r="D4" s="10">
         <f>C4+(C4*0.5)</f>
-        <v>2700</v>
+        <v>4320</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="19.95" customHeight="1">
@@ -2194,13 +2231,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.95" customHeight="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
     </row>
@@ -2266,8 +2303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1E3BF37-ABBD-4638-83D5-46916026A23D}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="19.95" customHeight="1"/>
@@ -2282,19 +2319,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.95" customHeight="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
     </row>
     <row r="2" spans="1:11" s="8" customFormat="1" ht="19.95" customHeight="1">
       <c r="A2" s="8" t="s">
@@ -2402,8 +2439,39 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="19.95" customHeight="1">
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="A5" s="16">
+        <v>8</v>
+      </c>
+      <c r="B5" s="16">
+        <v>7</v>
+      </c>
+      <c r="C5" s="17">
+        <v>8</v>
+      </c>
+      <c r="D5" s="17">
+        <v>2</v>
+      </c>
+      <c r="E5" s="11">
+        <v>3.9</v>
+      </c>
+      <c r="F5" s="13">
+        <v>1.89</v>
+      </c>
+      <c r="G5" s="16">
+        <v>1</v>
+      </c>
+      <c r="H5" s="16">
+        <v>1</v>
+      </c>
+      <c r="I5" s="7">
+        <v>6.4</v>
+      </c>
+      <c r="J5" s="7">
+        <v>0</v>
+      </c>
+      <c r="K5" s="7">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2435,15 +2503,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.95" customHeight="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" ht="19.95" customHeight="1">
       <c r="A2" s="2" t="s">
@@ -2528,10 +2596,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64DC4204-802F-419F-912A-BFCDF82124A2}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView zoomScale="63" zoomScaleNormal="63" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="19.95" customHeight="1"/>
@@ -2545,12 +2613,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.95" customHeight="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
@@ -2585,6 +2653,20 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" ht="19.95" customHeight="1">
+      <c r="A4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="1">
+        <v>5360.99</v>
+      </c>
+      <c r="C4" s="1">
+        <v>30</v>
+      </c>
+      <c r="D4" s="1">
+        <v>6969.29</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2600,10 +2682,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{318192DF-F290-435E-8F61-6C97D0171C4C}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView zoomScale="63" zoomScaleNormal="63" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="19.95" customHeight="1"/>
@@ -2617,12 +2699,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.95" customHeight="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
@@ -2657,6 +2739,20 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" ht="19.95" customHeight="1">
+      <c r="A4" s="1">
+        <v>28</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45</v>
+      </c>
+      <c r="C4" s="1">
+        <v>7808.39</v>
+      </c>
+      <c r="D4" s="1">
+        <v>13508.51</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2672,10 +2768,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53C51E04-357E-48C5-8E06-90D699CC3CBB}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView zoomScale="63" zoomScaleNormal="63" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="19.95" customHeight="1"/>
@@ -2689,13 +2785,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.95" customHeight="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
     </row>
@@ -2734,6 +2830,23 @@
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" ht="19.95" customHeight="1">
+      <c r="A4" s="1">
+        <v>3600</v>
+      </c>
+      <c r="B4" s="1">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1">
+        <v>150000</v>
+      </c>
+      <c r="D4" s="1">
+        <v>450</v>
+      </c>
+      <c r="E4" s="5">
+        <v>15600</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2749,10 +2862,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A83F9214-FAC2-44F4-B749-EE6235CD81F8}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView zoomScale="63" zoomScaleNormal="63" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="19.95" customHeight="1"/>
@@ -2766,10 +2879,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="19.95" customHeight="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="20"/>
+      <c r="B1" s="19"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -2792,6 +2905,14 @@
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" ht="19.95" customHeight="1">
+      <c r="A4" s="1">
+        <v>122</v>
+      </c>
+      <c r="B4" s="1">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2824,10 +2945,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="19.95" customHeight="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="20"/>
+      <c r="B1" s="19"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -2890,10 +3011,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="19.95" customHeight="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="20"/>
+      <c r="B1" s="19"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -2956,10 +3077,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="19.95" customHeight="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="20"/>
+      <c r="B1" s="19"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>

</xml_diff>